<commit_message>
push notification functionality working
</commit_message>
<xml_diff>
--- a/uploads/Round2_chessResultsList.xlsx
+++ b/uploads/Round2_chessResultsList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Bo.</t>
   </si>
@@ -93,225 +93,6 @@
     <t>1667</t>
   </si>
   <si>
-    <t>Walde Harshal</t>
-  </si>
-  <si>
-    <t>1652</t>
-  </si>
-  <si>
-    <t>MH</t>
-  </si>
-  <si>
-    <t>FM</t>
-  </si>
-  <si>
-    <t>Potawad Anirudhha</t>
-  </si>
-  <si>
-    <t>2288</t>
-  </si>
-  <si>
-    <t>Sangma Rahul</t>
-  </si>
-  <si>
-    <t>2136</t>
-  </si>
-  <si>
-    <t>GJ-RSPB</t>
-  </si>
-  <si>
-    <t>Pardeshi Chaturthi</t>
-  </si>
-  <si>
-    <t>F13</t>
-  </si>
-  <si>
-    <t>1661</t>
-  </si>
-  <si>
-    <t>Shinde Kunal</t>
-  </si>
-  <si>
-    <t>1644</t>
-  </si>
-  <si>
-    <t>Bhosale Shriraj</t>
-  </si>
-  <si>
-    <t>2113</t>
-  </si>
-  <si>
-    <t>Madkar Atharva</t>
-  </si>
-  <si>
-    <t>1976</t>
-  </si>
-  <si>
-    <t>Ishan Arjun P Y</t>
-  </si>
-  <si>
-    <t>U11</t>
-  </si>
-  <si>
-    <t>1647</t>
-  </si>
-  <si>
-    <t>Jathar Rishabh</t>
-  </si>
-  <si>
-    <t>1635</t>
-  </si>
-  <si>
-    <t>Aditya Savalkar</t>
-  </si>
-  <si>
-    <t>1927</t>
-  </si>
-  <si>
-    <t>Raghav Renuk Pawade</t>
-  </si>
-  <si>
-    <t>1620</t>
-  </si>
-  <si>
-    <t>Amartya Saumitra Gupta</t>
-  </si>
-  <si>
-    <t>U15</t>
-  </si>
-  <si>
-    <t>1878</t>
-  </si>
-  <si>
-    <t>DL</t>
-  </si>
-  <si>
-    <t>Kabnurakar Rushikesh</t>
-  </si>
-  <si>
-    <t>1865</t>
-  </si>
-  <si>
-    <t>Undale Shravni</t>
-  </si>
-  <si>
-    <t>1643</t>
-  </si>
-  <si>
-    <t>Menon Padmanand</t>
-  </si>
-  <si>
-    <t>1618</t>
-  </si>
-  <si>
-    <t>Patil Divya</t>
-  </si>
-  <si>
-    <t>1853</t>
-  </si>
-  <si>
-    <t>Rane Viraj</t>
-  </si>
-  <si>
-    <t>1840</t>
-  </si>
-  <si>
-    <t>Patil Disha</t>
-  </si>
-  <si>
-    <t>1633</t>
-  </si>
-  <si>
-    <t>Bathina Mokshatra Sri Abhiram</t>
-  </si>
-  <si>
-    <t>1594</t>
-  </si>
-  <si>
-    <t>AP-UIN</t>
-  </si>
-  <si>
-    <t>Raposo Maxwell</t>
-  </si>
-  <si>
-    <t>1838</t>
-  </si>
-  <si>
-    <t>GA</t>
-  </si>
-  <si>
-    <t>Kamble Dipankar</t>
-  </si>
-  <si>
-    <t>1584</t>
-  </si>
-  <si>
-    <t>Apurv Shekhar Desmukh</t>
-  </si>
-  <si>
-    <t>1806</t>
-  </si>
-  <si>
-    <t>Jadhav Omkar S</t>
-  </si>
-  <si>
-    <t>1574</t>
-  </si>
-  <si>
-    <t>Soni Deepak R</t>
-  </si>
-  <si>
-    <t>1770</t>
-  </si>
-  <si>
-    <t>Joshi Abhijeet</t>
-  </si>
-  <si>
-    <t>1756</t>
-  </si>
-  <si>
-    <t>AFM</t>
-  </si>
-  <si>
-    <t>Waghle Bhumika</t>
-  </si>
-  <si>
-    <t>F11</t>
-  </si>
-  <si>
-    <t>1619</t>
-  </si>
-  <si>
-    <t>ACM</t>
-  </si>
-  <si>
-    <t>Sudhan Deo</t>
-  </si>
-  <si>
-    <t>1571</t>
-  </si>
-  <si>
-    <t>Jagadale Ishwari</t>
-  </si>
-  <si>
-    <t>1755</t>
-  </si>
-  <si>
-    <t>Lokhandkar Rushikesh</t>
-  </si>
-  <si>
-    <t>1559</t>
-  </si>
-  <si>
-    <t>Kulkarni Nilay</t>
-  </si>
-  <si>
-    <t>1752</t>
-  </si>
-  <si>
-    <t>White-Username</t>
-  </si>
-  <si>
     <t>Black-UserName</t>
   </si>
   <si>
@@ -327,7 +108,7 @@
     <t>Harsh27</t>
   </si>
   <si>
-    <t>Soham</t>
+    <t>White-UserName</t>
   </si>
 </sst>
 </file>
@@ -6798,7 +6579,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6830,7 +6611,7 @@
       <c r="B1" s="4"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -6855,7 +6636,7 @@
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>7</v>
@@ -6880,7 +6661,7 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
@@ -6907,7 +6688,7 @@
         <v>14</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>15</v>
@@ -6934,7 +6715,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>18</v>
@@ -6957,7 +6738,7 @@
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>22</v>
@@ -6974,690 +6755,304 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1</v>
-      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="2">
-        <v>1</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1</v>
-      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="2">
-        <v>1</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="2">
-        <v>1</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13" s="2">
-        <v>1</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1</v>
-      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="2">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="2">
-        <v>1</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1</v>
-      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>88</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1</v>
-      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="2">
-        <v>1</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1</v>
-      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1" t="s">
-        <v>94</v>
-      </c>
+      <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>